<commit_message>
Updated params excel file
</commit_message>
<xml_diff>
--- a/parameters_file_single_ASE_AP5GC.xlsx
+++ b/parameters_file_single_ASE_AP5GC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudeepch\Downloads\ASE_automated_deployment\ASE_automated_deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/sudeepch_microsoft_com/Documents/Documents/GitHub/ASE_automation_for_AP5GC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C711A6B7-A73A-4074-945D-41841193E008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{C711A6B7-A73A-4074-945D-41841193E008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D93E6653-CFD5-49C0-967F-469103FAD284}"/>
   <bookViews>
-    <workbookView xWindow="75720" yWindow="3090" windowWidth="38640" windowHeight="21120" xr2:uid="{54FBBA50-3CB6-49FD-BB52-63DFE9B337B6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{54FBBA50-3CB6-49FD-BB52-63DFE9B337B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -647,9 +647,6 @@
     <t>trustSelfSignedCertificate</t>
   </si>
   <si>
-    <t>crlL5n0enXH@Lry</t>
-  </si>
-  <si>
     <t>8698f174-10b0-4e39-9ddb-9ded1839200b</t>
   </si>
   <si>
@@ -678,6 +675,9 @@
   </si>
   <si>
     <t>custom-loc6-mcn2</t>
+  </si>
+  <si>
+    <t>&lt;Enter current ASE password&gt;</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1129,7 @@
   <dimension ref="A1:D112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1173,7 +1173,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>167</v>
@@ -1187,7 +1187,7 @@
         <v>202</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C4" s="9" t="b">
         <v>0</v>
@@ -1213,7 +1213,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>83</v>
@@ -1241,7 +1241,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>171</v>
@@ -2295,7 +2295,7 @@
         <v>62</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>186</v>
@@ -2319,7 +2319,7 @@
         <v>19</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>185</v>
@@ -2379,7 +2379,7 @@
         <v>67</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C99" s="5"/>
       <c r="D99" s="3"/>
@@ -2389,7 +2389,7 @@
         <v>68</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C100" s="5"/>
       <c r="D100" s="3"/>
@@ -2399,7 +2399,7 @@
         <v>69</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
@@ -2459,7 +2459,7 @@
         <v>76</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
@@ -2469,7 +2469,7 @@
         <v>77</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>

</xml_diff>

<commit_message>
corrected the Port2 blocks in the Diagram worksheet
</commit_message>
<xml_diff>
--- a/parameters_file_single_ASE_AP5GC.xlsx
+++ b/parameters_file_single_ASE_AP5GC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/sudeepch_microsoft_com/Documents/Documents/GitHub/ASE_automation_for_AP5GC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{9766DEE8-3A80-4B05-803E-92A8B2C526CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F8E35FB-BA80-4061-A74C-82920E856FB0}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{9766DEE8-3A80-4B05-803E-92A8B2C526CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0B7AFEF-9A2B-4886-A746-BED69FA91170}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{54FBBA50-3CB6-49FD-BB52-63DFE9B337B6}"/>
+    <workbookView xWindow="75720" yWindow="3090" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{54FBBA50-3CB6-49FD-BB52-63DFE9B337B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Datafill" sheetId="1" r:id="rId1"/>
@@ -1492,1766 +1492,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="70" name="Group 69" descr="A graphical representation of the values supplied in the datafill sheet, such as IP addressing and ports.">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33CBA197-6610-B6DC-96C5-240BBC71F1CE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="4702175" y="161925"/>
-          <a:ext cx="9744075" cy="4556125"/>
-          <a:chOff x="4162425" y="600075"/>
-          <a:chExt cx="9744075" cy="4714875"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="Datafill!B9">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="2" name="Rectangle 1">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5FBC81B-29F9-9456-B90B-734C8D8325C3}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4162425" y="600075"/>
-            <a:ext cx="9744075" cy="4714875"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{3DFE34C5-411A-4C2C-8830-C5A3D89E233F}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:schemeClr val="bg2"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>CONTOSO-AP5GC5G-ASE02-ASE</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="bg2"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="22" name="Rectangle: Rounded Corners 21">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0682508F-3F98-969D-4F48-613BD7EC2DF7}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4914900" y="3181350"/>
-            <a:ext cx="8601075" cy="1905000"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent2">
-              <a:alpha val="94000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$1">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Rectangle 2">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F197C56-920D-C8E8-EA17-CC8081011CC2}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4581526" y="695325"/>
-            <a:ext cx="1352550" cy="466725"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{D0E77798-01AA-4CF6-BF92-897D94D81EF4}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>Port 1: 10.214.5.20</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$2">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Rectangle 3">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E6D547F-B77C-4D48-8036-B354703D8809}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6296026" y="657224"/>
-            <a:ext cx="1762124" cy="809625"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{B0272850-A296-4447-856C-5E1827D4CEF2}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>Port 2: 
-192.168.105.0
-Subnet 255.255.255.0
- Gateway: 192.168.105.1</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$3">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Rectangle 4">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4604A1E8-5B58-44E8-80D9-9463BEB5381A}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="8315326" y="676275"/>
-            <a:ext cx="1743074" cy="800100"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{52BA3796-1BFC-4EE3-A0ED-5E3E3699C9F7}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>Port 3: 
-192.168.105.0
-Subnet 255.255.255.0
- Gateway: 192.168.105.1</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$4">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="Rectangle 5">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B7B3A0D-E5DB-4BA8-93C1-A313B961CC3D}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="11039476" y="695325"/>
-            <a:ext cx="1838324" cy="800100"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{EEF2E7F5-2B4C-4163-A729-B12DB79C8901}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>Port 4: 
-192.168.106.0
-Subnet 255.255.255.0
- Gateway: 192.168.106.1</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$5">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="Rectangle 7">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA74B1C2-97A3-4A3A-BDFC-8F6784778E21}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6505575" y="1685926"/>
-            <a:ext cx="1352550" cy="304800"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{061D4A8F-F2A1-4B7B-9071-1E2CF347D276}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>vswitch-port2</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$6">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="9" name="Rectangle 8">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEC969B1-1A4B-44C0-A1EA-673BA6572310}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="8515350" y="1695450"/>
-            <a:ext cx="1352550" cy="295275"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{B2B5B0F1-B408-454B-A133-669F3E5F14AE}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>vswitch-port3</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$7">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="Rectangle 9">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A997C9A-DBCF-44EB-B49E-971140176202}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="11287125" y="1724025"/>
-            <a:ext cx="1352550" cy="295275"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{6E7B82F5-F7B6-4AF1-BD40-3DD735B2D070}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>vswitch-port4</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$8">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="11" name="Rectangle 10">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2D55651-7B5C-4821-BE8A-51EF0483C194}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7600950" y="2352675"/>
-            <a:ext cx="1352550" cy="466725"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{3B64F593-E8E0-462B-9CF0-5742325CC82F}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>N2
-IP: 192.168.105.22</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$9">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="12" name="Rectangle 11">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18F53733-FE24-425B-8317-FFBF8800CFBA}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9144000" y="2352675"/>
-            <a:ext cx="1352550" cy="466725"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{64393C8B-C181-4BFB-91E1-C51FFD660700}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>N3
-IP: 192.168.105.23</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$10">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="13" name="Rectangle 12">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A315B33-7EE8-4547-B9CA-2AC2D8EC6901}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="10820400" y="2247899"/>
-            <a:ext cx="2286000" cy="828675"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{FAB59671-4B78-4BC4-B184-F122FB49135B}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>Total Number of DNNs: 10
-N6-DNN1
-VLAN: 666
-IP 192.168.106.0 / 255.255.255.0</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$11">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="14" name="Rectangle 13">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65DF9E79-C354-4B9E-982D-9008C2413723}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5781675" y="4029075"/>
-            <a:ext cx="1714500" cy="466725"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{FE782CF8-74B5-442A-AD25-DF53ACDDE059}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>K8s Node IP Range: 10.214.5.21-10.214.5.26</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$12">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="15" name="Rectangle 14">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E354E4B4-8485-42FC-AADE-92E8BE43ED4E}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5400675" y="3438525"/>
-            <a:ext cx="1733550" cy="447675"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{981684E2-0713-456A-AF90-5DB2B29F0C8A}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>K8s External (Grafana/SAS): 10.214.5.27-10.214.5.27</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$13">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="16" name="Rectangle 15">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC55A3AC-897A-47C6-B447-9AC4E6142668}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7620000" y="3648075"/>
-            <a:ext cx="1352550" cy="466725"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{F8DC2631-E6EB-41EA-9E1D-10EBE3283DC3}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>N2/MME IP: 192.168.105.22</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$14">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="17" name="Rectangle 16">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D214B680-184A-4B93-91E2-3F6652BDF110}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9153525" y="3648075"/>
-            <a:ext cx="1352550" cy="466725"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{B971E119-C564-427B-A094-A82AB063DE9D}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>N3/SI-U IP: 192.168.105.23</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$15">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="18" name="Rectangle 17">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A851C90-A657-4EA8-8B9D-A48BA4AC0FC1}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="10763250" y="3486150"/>
-            <a:ext cx="2438400" cy="457200"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{65964BB4-A79D-4B04-B30D-DEB91D192E9E}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>N6/SGi IP: 192.168.106.36
-(N6-DNN1)</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$16">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="19" name="Rectangle 18">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF5E44A3-C428-457F-98DB-DAE8E3825593}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="8372475" y="4552950"/>
-            <a:ext cx="1352550" cy="466725"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent3">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent3"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent3"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{053D4BFE-DA8C-43DC-8AB0-8E30F69197A9}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:schemeClr val="bg2"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>PLMN: 999/99
-Mode: EPC + 5GC</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="bg2"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$17">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="20" name="Rectangle 19">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A60A216D-951F-43F6-9B18-FE4C1E33D74B}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="10791824" y="4257676"/>
-            <a:ext cx="2390775" cy="285750"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{A68D1ACB-095D-48F5-A3E5-BB5400CA0CD0}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>Dynamic UE IPs: 192.168.50.0/24</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$18">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="21" name="Rectangle 20">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{576C534C-B031-484A-B739-B4855A8148FE}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="10791824" y="4610101"/>
-            <a:ext cx="2390775" cy="285750"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{B6D13742-81B7-4DE5-A16B-903D4579AA29}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>Static UE IPs: 192.168.60.0/24</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="24" name="Straight Connector 23">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C762AA9-8B35-C9FE-0F7A-59BEA9C58B58}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="4" idx="2"/>
-            <a:endCxn id="8" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7177088" y="1466849"/>
-            <a:ext cx="4762" cy="219077"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="27" name="Straight Connector 26">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98054823-F876-4217-8853-843CACEB6AF0}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="5" idx="2"/>
-            <a:endCxn id="9" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9186863" y="1476375"/>
-            <a:ext cx="4762" cy="219075"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="31" name="Straight Connector 30">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3459C8AE-A4E8-4A62-BA97-B08C0B87092C}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="8" idx="2"/>
-            <a:endCxn id="15" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1">
-            <a:off x="6267450" y="1990726"/>
-            <a:ext cx="914400" cy="1447799"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="32" name="Straight Connector 31">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51681B27-C4C6-42FB-9B01-E882B497A224}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="6" idx="2"/>
-            <a:endCxn id="10" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="11958638" y="1495425"/>
-            <a:ext cx="4762" cy="228600"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="40" name="Straight Connector 39">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52EE9014-458F-4F49-B336-1486F3AB7404}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="8" idx="2"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7181850" y="1990726"/>
-            <a:ext cx="114300" cy="2047874"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="43" name="Straight Connector 42">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEF5024B-F6D6-4F4A-9CCA-3E92AAB7BD31}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="9" idx="2"/>
-            <a:endCxn id="11" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1">
-            <a:off x="8277225" y="1990725"/>
-            <a:ext cx="914400" cy="361950"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="46" name="Straight Connector 45">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7512639-D2E8-4A64-A14B-4C17B5F9E1FC}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="9" idx="2"/>
-            <a:endCxn id="12" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9191625" y="1990725"/>
-            <a:ext cx="628650" cy="361950"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="49" name="Straight Connector 48">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E6B8E0-FAED-4340-8CD6-A804C221463C}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="10" idx="2"/>
-            <a:endCxn id="13" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="11963400" y="2019300"/>
-            <a:ext cx="0" cy="228599"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="52" name="Straight Connector 51">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1FEF420-5973-4BAD-B309-090E6F73BCBA}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="12" idx="2"/>
-            <a:endCxn id="17" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9820275" y="2819400"/>
-            <a:ext cx="9525" cy="828675"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="55" name="Straight Connector 54">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE549540-226E-48F4-B574-BAA5477C44E7}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="11" idx="2"/>
-            <a:endCxn id="16" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="8277225" y="2819400"/>
-            <a:ext cx="19050" cy="828675"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="58" name="Straight Connector 57">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC356EB-356A-4A6D-BDF9-75E3D1F46448}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="13" idx="2"/>
-            <a:endCxn id="18" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="11963400" y="3076574"/>
-            <a:ext cx="19050" cy="409576"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="61" name="Straight Connector 60">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85822DEC-A144-4855-A1C9-08AF470DBAF9}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="20" idx="0"/>
-            <a:endCxn id="18" idx="2"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1" flipV="1">
-            <a:off x="11982450" y="3943350"/>
-            <a:ext cx="4762" cy="314326"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="64" name="Rectangle: Rounded Corners 63">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA443779-3A89-99AF-5007-B531058A66B6}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4848225" y="1409700"/>
-            <a:ext cx="828675" cy="390525"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:lnRef>
-          <a:fillRef idx="2">
-            <a:schemeClr val="accent6"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent6"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-US" sz="1100"/>
-              <a:t>ASE UI</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="65" name="Straight Connector 64">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D0BAD51-4AFF-4ADC-98AD-F0036EFEF2A3}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr>
-            <a:stCxn id="3" idx="2"/>
-            <a:endCxn id="64" idx="0"/>
-          </xdr:cNvCxnSpPr>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5257801" y="1162050"/>
-            <a:ext cx="4762" cy="247650"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="$A$19">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="69" name="Rectangle: Rounded Corners 68">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1691EB72-9358-97B5-BE4E-1F67837EA39F}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5981699" y="4714875"/>
-            <a:ext cx="1838325" cy="295275"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg2"/>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:fld id="{44DE0CF8-B28E-456B-88C7-EFAF942A54F5}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="l"/>
-              <a:t>Site Name: CONTOSO-SITE-CO</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>165099</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:colOff>174624</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>333374</xdr:colOff>
+      <xdr:colOff>342899</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -3266,8 +1515,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4705349" y="158750"/>
-          <a:ext cx="16017875" cy="7680325"/>
+          <a:off x="4718049" y="180975"/>
+          <a:ext cx="16017875" cy="7540625"/>
           <a:chOff x="4162425" y="600075"/>
           <a:chExt cx="9744075" cy="4714875"/>
         </a:xfrm>
@@ -3383,10 +1632,10 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="$A$1">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="94" name="Rectangle 93">
+          <xdr:cNvPr id="95" name="Rectangle 94">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4294CFB5-83E5-E4B4-34AC-CE7C802C4E42}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E9B1CAD-0855-4E97-0A0F-FE8FDE862F9C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3394,8 +1643,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4581526" y="695325"/>
-            <a:ext cx="1352550" cy="466725"/>
+            <a:off x="6296026" y="675077"/>
+            <a:ext cx="1762124" cy="335923"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -3422,73 +1671,15 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:fld id="{D0E77798-01AA-4CF6-BF92-897D94D81EF4}" type="TxLink">
+            <a:fld id="{A54D23CD-C093-4977-B76A-2547F1A501AF}" type="TxLink">
               <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
               </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>Port 1: 10.214.5.20</a:t>
-            </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="$A$2">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="95" name="Rectangle 94">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E9B1CAD-0855-4E97-0A0F-FE8FDE862F9C}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6296026" y="657224"/>
-            <a:ext cx="1762124" cy="809625"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent4">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent4"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent4"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:fld id="{B0272850-A296-4447-856C-5E1827D4CEF2}" type="TxLink">
-              <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Aptos Narrow"/>
-              </a:rPr>
-              <a:pPr algn="ctr"/>
-              <a:t>Port 2: 
-192.168.105.0
-Subnet 255.255.255.0
- Gateway: 192.168.105.1</a:t>
+              <a:t>Port2
+IP: 10.214.5.20</a:t>
             </a:fld>
             <a:endParaRPr lang="en-US" sz="1100"/>
           </a:p>
@@ -4407,8 +2598,8 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="7177088" y="1466849"/>
-            <a:ext cx="4762" cy="219077"/>
+            <a:off x="7177088" y="1011000"/>
+            <a:ext cx="4762" cy="674926"/>
           </a:xfrm>
           <a:prstGeom prst="line">
             <a:avLst/>
@@ -4859,7 +3050,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="4848225" y="1409700"/>
+            <a:off x="4894580" y="700930"/>
             <a:ext cx="828675" cy="390525"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
@@ -4902,14 +3093,14 @@
             </a:extLst>
           </xdr:cNvPr>
           <xdr:cNvCxnSpPr>
-            <a:stCxn id="94" idx="2"/>
-            <a:endCxn id="124" idx="0"/>
+            <a:cxnSpLocks/>
+            <a:stCxn id="95" idx="1"/>
           </xdr:cNvCxnSpPr>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5257801" y="1162050"/>
-            <a:ext cx="4762" cy="247650"/>
+          <a:xfrm flipH="1">
+            <a:off x="5742337" y="843039"/>
+            <a:ext cx="553689" cy="13021"/>
           </a:xfrm>
           <a:prstGeom prst="line">
             <a:avLst/>
@@ -6115,15 +4306,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>187194</xdr:colOff>
+      <xdr:colOff>193544</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>141366</xdr:rowOff>
+      <xdr:rowOff>163591</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:colOff>225425</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -6140,7 +4331,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17529044" y="4125991"/>
+          <a:off x="17538569" y="4145041"/>
           <a:ext cx="641481" cy="519034"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -6760,11 +4951,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8373,8 +6564,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8384,8 +6575,9 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="str">
-        <f>"Port 1: " &amp; ASEip</f>
-        <v>Port 1: 10.214.5.20</v>
+        <f>vSwitchMgmtPortAlias &amp; CHAR(10) &amp; "IP: " &amp; ASEip</f>
+        <v>Port2
+IP: 10.214.5.20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
updated parameters file with latest 2403 script, includes SkipLogin option
</commit_message>
<xml_diff>
--- a/parameters_file_single_ASE_AP5GC.xlsx
+++ b/parameters_file_single_ASE_AP5GC.xlsx
@@ -1,133 +1,133 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/sudeepch_microsoft_com/Documents/Documents/GitHub/ASE_automation_for_AP5GC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{9766DEE8-3A80-4B05-803E-92A8B2C526CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0B7AFEF-9A2B-4886-A746-BED69FA91170}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{F3EF7CE0-A92A-4BD7-8994-34C8F583455B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83389669-A311-4D6D-A464-79E4E73ED8C8}"/>
   <bookViews>
-    <workbookView xWindow="75720" yWindow="3090" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{54FBBA50-3CB6-49FD-BB52-63DFE9B337B6}"/>
+    <workbookView xWindow="37320" yWindow="3045" windowWidth="38640" windowHeight="21120" xr2:uid="{54FBBA50-3CB6-49FD-BB52-63DFE9B337B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Datafill" sheetId="1" r:id="rId1"/>
     <sheet name="Diagram" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="arcClusterName">Datafill!$B$10</definedName>
-    <definedName name="arcLocation">Datafill!$B$12</definedName>
+    <definedName name="arcClusterName">Datafill!$B$11</definedName>
+    <definedName name="arcLocation">Datafill!$B$13</definedName>
     <definedName name="ASEip">Datafill!$B$2</definedName>
-    <definedName name="ASEresourceGroup">Datafill!$B$8</definedName>
-    <definedName name="azureStackEdgeDevice">Datafill!$B$9</definedName>
-    <definedName name="computeKubernetesNodeIps">Datafill!$B$15</definedName>
-    <definedName name="computeKubernetesServiceIps">Datafill!$B$16</definedName>
-    <definedName name="coreNetworkTechnology">Datafill!$B$29</definedName>
-    <definedName name="customLocationName">Datafill!$B$11</definedName>
-    <definedName name="dataNetworkName">Datafill!$B$43</definedName>
+    <definedName name="ASEresourceGroup">Datafill!$B$9</definedName>
+    <definedName name="azureStackEdgeDevice">Datafill!$B$10</definedName>
+    <definedName name="computeKubernetesNodeIps">Datafill!$B$16</definedName>
+    <definedName name="computeKubernetesServiceIps">Datafill!$B$17</definedName>
+    <definedName name="coreNetworkTechnology">Datafill!$B$30</definedName>
+    <definedName name="customLocationName">Datafill!$B$12</definedName>
+    <definedName name="dataNetworkName">Datafill!$B$44</definedName>
     <definedName name="defaultASEPassword">Datafill!$B$3</definedName>
-    <definedName name="dnsAddresses">Datafill!$B$106</definedName>
-    <definedName name="location">Datafill!$B$26</definedName>
-    <definedName name="mobileCountryCode">Datafill!$B$24</definedName>
-    <definedName name="mobileNetworkCode">Datafill!$B$25</definedName>
-    <definedName name="mobileNetworkName">Datafill!$B$22</definedName>
-    <definedName name="mobileNetworkRGName">Datafill!$B$23</definedName>
-    <definedName name="mobileNetworkRGNameLocation">Datafill!$B$27</definedName>
-    <definedName name="mtuASE">Datafill!$B$21</definedName>
-    <definedName name="n2Gateway">Datafill!$B$34</definedName>
-    <definedName name="n2IP">Datafill!$B$35</definedName>
-    <definedName name="n2Network">Datafill!$B$33</definedName>
-    <definedName name="n2SubnetMask">Datafill!$B$32</definedName>
-    <definedName name="N2vlanId">Datafill!$B$31</definedName>
-    <definedName name="N2vSwitchName">Datafill!$B$30</definedName>
-    <definedName name="n3Gateway">Datafill!$B$40</definedName>
-    <definedName name="n3IP">Datafill!$B$41</definedName>
-    <definedName name="n3Network">Datafill!$B$39</definedName>
-    <definedName name="n3SubnetMask">Datafill!$B$38</definedName>
-    <definedName name="N3vlanId">Datafill!$B$37</definedName>
-    <definedName name="N3vSwitchName">Datafill!$B$36</definedName>
-    <definedName name="N6DNN10vSwitchName">Datafill!$B$54</definedName>
-    <definedName name="N6DNN1vSwitchName">Datafill!$B$45</definedName>
-    <definedName name="N6DNN2vSwitchName">Datafill!$B$46</definedName>
-    <definedName name="N6DNN3vSwitchName">Datafill!$B$47</definedName>
-    <definedName name="N6DNN4vSwitchName">Datafill!$B$48</definedName>
-    <definedName name="N6DNN5vSwitchName">Datafill!$B$49</definedName>
-    <definedName name="N6DNN6vSwitchName">Datafill!$B$50</definedName>
-    <definedName name="N6DNN7vSwitchName">Datafill!$B$51</definedName>
-    <definedName name="N6DNN8vSwitchName">Datafill!$B$52</definedName>
-    <definedName name="N6DNN9vSwitchName">Datafill!$B$53</definedName>
-    <definedName name="n6GatewayDNN1">Datafill!$B$85</definedName>
-    <definedName name="n6GatewayDNN10">Datafill!$B$94</definedName>
-    <definedName name="n6GatewayDNN2">Datafill!$B$86</definedName>
-    <definedName name="n6GatewayDNN3">Datafill!$B$87</definedName>
-    <definedName name="n6GatewayDNN4">Datafill!$B$88</definedName>
-    <definedName name="n6GatewayDNN5">Datafill!$B$89</definedName>
-    <definedName name="n6GatewayDNN6">Datafill!$B$90</definedName>
-    <definedName name="n6GatewayDNN7">Datafill!$B$91</definedName>
-    <definedName name="n6GatewayDNN8">Datafill!$B$92</definedName>
-    <definedName name="n6GatewayDNN9">Datafill!$B$93</definedName>
-    <definedName name="n6IPDNN1">Datafill!$B$75</definedName>
-    <definedName name="n6IPDNN10">Datafill!$B$84</definedName>
-    <definedName name="n6IPDNN2">Datafill!$B$76</definedName>
-    <definedName name="n6IPDNN3">Datafill!$B$77</definedName>
-    <definedName name="n6IPDNN4">Datafill!$B$78</definedName>
-    <definedName name="n6IPDNN5">Datafill!$B$79</definedName>
-    <definedName name="n6IPDNN6">Datafill!$B$80</definedName>
-    <definedName name="n6IPDNN7">Datafill!$B$81</definedName>
-    <definedName name="n6IPDNN8">Datafill!$B$82</definedName>
-    <definedName name="n6IPDNN9">Datafill!$B$83</definedName>
-    <definedName name="n6NetworkDNN1">Datafill!$B$65</definedName>
-    <definedName name="n6NetworkDNN10">Datafill!$B$74</definedName>
-    <definedName name="n6NetworkDNN2">Datafill!$B$66</definedName>
-    <definedName name="n6NetworkDNN3">Datafill!$B$67</definedName>
-    <definedName name="n6NetworkDNN4">Datafill!$B$68</definedName>
-    <definedName name="n6NetworkDNN5">Datafill!$B$69</definedName>
-    <definedName name="n6NetworkDNN6">Datafill!$B$70</definedName>
-    <definedName name="n6NetworkDNN7">Datafill!$B$71</definedName>
-    <definedName name="n6NetworkDNN8">Datafill!$B$72</definedName>
-    <definedName name="n6NetworkDNN9">Datafill!$B$73</definedName>
-    <definedName name="n6SubnetMaskDNN1">Datafill!$B$55</definedName>
-    <definedName name="n6SubnetMaskDNN10">Datafill!$B$64</definedName>
-    <definedName name="n6SubnetMaskDNN2">Datafill!$B$56</definedName>
-    <definedName name="n6SubnetMaskDNN3">Datafill!$B$57</definedName>
-    <definedName name="n6SubnetMaskDNN4">Datafill!$B$58</definedName>
-    <definedName name="n6SubnetMaskDNN5">Datafill!$B$59</definedName>
-    <definedName name="n6SubnetMaskDNN6">Datafill!$B$60</definedName>
-    <definedName name="n6SubnetMaskDNN7">Datafill!$B$61</definedName>
-    <definedName name="n6SubnetMaskDNN8">Datafill!$B$62</definedName>
-    <definedName name="n6SubnetMaskDNN9">Datafill!$B$63</definedName>
-    <definedName name="N6vlanIdDNN1">Datafill!$B$95</definedName>
-    <definedName name="N6vlanIdDNN10">Datafill!$B$104</definedName>
-    <definedName name="N6vlanIdDNN2">Datafill!$B$96</definedName>
-    <definedName name="N6vlanIdDNN3">Datafill!$B$97</definedName>
-    <definedName name="N6vlanIdDNN4">Datafill!$B$98</definedName>
-    <definedName name="N6vlanIdDNN5">Datafill!$B$99</definedName>
-    <definedName name="N6vlanIdDNN6">Datafill!$B$100</definedName>
-    <definedName name="N6vlanIdDNN7">Datafill!$B$101</definedName>
-    <definedName name="N6vlanIdDNN8">Datafill!$B$102</definedName>
-    <definedName name="N6vlanIdDNN9">Datafill!$B$103</definedName>
-    <definedName name="naptEnabled">Datafill!$B$105</definedName>
-    <definedName name="numberofDNNs">Datafill!$B$42</definedName>
-    <definedName name="oid">Datafill!$B$5</definedName>
-    <definedName name="serviceName">Datafill!$B$109</definedName>
-    <definedName name="simGroupName">Datafill!$B$112</definedName>
-    <definedName name="simPolicyName">Datafill!$B$110</definedName>
-    <definedName name="siteName">Datafill!$B$28</definedName>
-    <definedName name="sliceName">Datafill!$B$111</definedName>
-    <definedName name="subscriptionId">Datafill!$B$6</definedName>
-    <definedName name="tenantId">Datafill!$B$7</definedName>
+    <definedName name="dnsAddresses">Datafill!$B$107</definedName>
+    <definedName name="location">Datafill!$B$27</definedName>
+    <definedName name="mobileCountryCode">Datafill!$B$25</definedName>
+    <definedName name="mobileNetworkCode">Datafill!$B$26</definedName>
+    <definedName name="mobileNetworkName">Datafill!$B$23</definedName>
+    <definedName name="mobileNetworkRGName">Datafill!$B$24</definedName>
+    <definedName name="mobileNetworkRGNameLocation">Datafill!$B$28</definedName>
+    <definedName name="mtuASE">Datafill!$B$22</definedName>
+    <definedName name="n2Gateway">Datafill!$B$35</definedName>
+    <definedName name="n2IP">Datafill!$B$36</definedName>
+    <definedName name="n2Network">Datafill!$B$34</definedName>
+    <definedName name="n2SubnetMask">Datafill!$B$33</definedName>
+    <definedName name="N2vlanId">Datafill!$B$32</definedName>
+    <definedName name="N2vSwitchName">Datafill!$B$31</definedName>
+    <definedName name="n3Gateway">Datafill!$B$41</definedName>
+    <definedName name="n3IP">Datafill!$B$42</definedName>
+    <definedName name="n3Network">Datafill!$B$40</definedName>
+    <definedName name="n3SubnetMask">Datafill!$B$39</definedName>
+    <definedName name="N3vlanId">Datafill!$B$38</definedName>
+    <definedName name="N3vSwitchName">Datafill!$B$37</definedName>
+    <definedName name="N6DNN10vSwitchName">Datafill!$B$55</definedName>
+    <definedName name="N6DNN1vSwitchName">Datafill!$B$46</definedName>
+    <definedName name="N6DNN2vSwitchName">Datafill!$B$47</definedName>
+    <definedName name="N6DNN3vSwitchName">Datafill!$B$48</definedName>
+    <definedName name="N6DNN4vSwitchName">Datafill!$B$49</definedName>
+    <definedName name="N6DNN5vSwitchName">Datafill!$B$50</definedName>
+    <definedName name="N6DNN6vSwitchName">Datafill!$B$51</definedName>
+    <definedName name="N6DNN7vSwitchName">Datafill!$B$52</definedName>
+    <definedName name="N6DNN8vSwitchName">Datafill!$B$53</definedName>
+    <definedName name="N6DNN9vSwitchName">Datafill!$B$54</definedName>
+    <definedName name="n6GatewayDNN1">Datafill!$B$86</definedName>
+    <definedName name="n6GatewayDNN10">Datafill!$B$95</definedName>
+    <definedName name="n6GatewayDNN2">Datafill!$B$87</definedName>
+    <definedName name="n6GatewayDNN3">Datafill!$B$88</definedName>
+    <definedName name="n6GatewayDNN4">Datafill!$B$89</definedName>
+    <definedName name="n6GatewayDNN5">Datafill!$B$90</definedName>
+    <definedName name="n6GatewayDNN6">Datafill!$B$91</definedName>
+    <definedName name="n6GatewayDNN7">Datafill!$B$92</definedName>
+    <definedName name="n6GatewayDNN8">Datafill!$B$93</definedName>
+    <definedName name="n6GatewayDNN9">Datafill!$B$94</definedName>
+    <definedName name="n6IPDNN1">Datafill!$B$76</definedName>
+    <definedName name="n6IPDNN10">Datafill!$B$85</definedName>
+    <definedName name="n6IPDNN2">Datafill!$B$77</definedName>
+    <definedName name="n6IPDNN3">Datafill!$B$78</definedName>
+    <definedName name="n6IPDNN4">Datafill!$B$79</definedName>
+    <definedName name="n6IPDNN5">Datafill!$B$80</definedName>
+    <definedName name="n6IPDNN6">Datafill!$B$81</definedName>
+    <definedName name="n6IPDNN7">Datafill!$B$82</definedName>
+    <definedName name="n6IPDNN8">Datafill!$B$83</definedName>
+    <definedName name="n6IPDNN9">Datafill!$B$84</definedName>
+    <definedName name="n6NetworkDNN1">Datafill!$B$66</definedName>
+    <definedName name="n6NetworkDNN10">Datafill!$B$75</definedName>
+    <definedName name="n6NetworkDNN2">Datafill!$B$67</definedName>
+    <definedName name="n6NetworkDNN3">Datafill!$B$68</definedName>
+    <definedName name="n6NetworkDNN4">Datafill!$B$69</definedName>
+    <definedName name="n6NetworkDNN5">Datafill!$B$70</definedName>
+    <definedName name="n6NetworkDNN6">Datafill!$B$71</definedName>
+    <definedName name="n6NetworkDNN7">Datafill!$B$72</definedName>
+    <definedName name="n6NetworkDNN8">Datafill!$B$73</definedName>
+    <definedName name="n6NetworkDNN9">Datafill!$B$74</definedName>
+    <definedName name="n6SubnetMaskDNN1">Datafill!$B$56</definedName>
+    <definedName name="n6SubnetMaskDNN10">Datafill!$B$65</definedName>
+    <definedName name="n6SubnetMaskDNN2">Datafill!$B$57</definedName>
+    <definedName name="n6SubnetMaskDNN3">Datafill!$B$58</definedName>
+    <definedName name="n6SubnetMaskDNN4">Datafill!$B$59</definedName>
+    <definedName name="n6SubnetMaskDNN5">Datafill!$B$60</definedName>
+    <definedName name="n6SubnetMaskDNN6">Datafill!$B$61</definedName>
+    <definedName name="n6SubnetMaskDNN7">Datafill!$B$62</definedName>
+    <definedName name="n6SubnetMaskDNN8">Datafill!$B$63</definedName>
+    <definedName name="n6SubnetMaskDNN9">Datafill!$B$64</definedName>
+    <definedName name="N6vlanIdDNN1">Datafill!$B$96</definedName>
+    <definedName name="N6vlanIdDNN10">Datafill!$B$105</definedName>
+    <definedName name="N6vlanIdDNN2">Datafill!$B$97</definedName>
+    <definedName name="N6vlanIdDNN3">Datafill!$B$98</definedName>
+    <definedName name="N6vlanIdDNN4">Datafill!$B$99</definedName>
+    <definedName name="N6vlanIdDNN5">Datafill!$B$100</definedName>
+    <definedName name="N6vlanIdDNN6">Datafill!$B$101</definedName>
+    <definedName name="N6vlanIdDNN7">Datafill!$B$102</definedName>
+    <definedName name="N6vlanIdDNN8">Datafill!$B$103</definedName>
+    <definedName name="N6vlanIdDNN9">Datafill!$B$104</definedName>
+    <definedName name="naptEnabled">Datafill!$B$106</definedName>
+    <definedName name="numberofDNNs">Datafill!$B$43</definedName>
+    <definedName name="oid">Datafill!$B$6</definedName>
+    <definedName name="serviceName">Datafill!$B$110</definedName>
+    <definedName name="simGroupName">Datafill!$B$113</definedName>
+    <definedName name="simPolicyName">Datafill!$B$111</definedName>
+    <definedName name="siteName">Datafill!$B$29</definedName>
+    <definedName name="sliceName">Datafill!$B$112</definedName>
+    <definedName name="subscriptionId">Datafill!$B$7</definedName>
+    <definedName name="tenantId">Datafill!$B$8</definedName>
     <definedName name="trustSelfSignedCertificate">Datafill!$B$4</definedName>
-    <definedName name="userEquipmentAddressPoolPrefix">Datafill!$B$107</definedName>
-    <definedName name="userEquipmentStaticAddressPoolPrefix">Datafill!$B$108</definedName>
-    <definedName name="userPlaneDataInterfaceName">Datafill!$B$44</definedName>
-    <definedName name="vSwitchACCESSPortAlias">Datafill!$B$18</definedName>
-    <definedName name="vSwitchACCESSPortName">Datafill!$B$17</definedName>
-    <definedName name="vSwitchDATAPortAlias">Datafill!$B$20</definedName>
-    <definedName name="vSwitchDATAPortName">Datafill!$B$19</definedName>
-    <definedName name="vSwitchMgmtPortAlias">Datafill!$B$14</definedName>
-    <definedName name="vSwitchMgmtPortName">Datafill!$B$13</definedName>
+    <definedName name="userEquipmentAddressPoolPrefix">Datafill!$B$108</definedName>
+    <definedName name="userEquipmentStaticAddressPoolPrefix">Datafill!$B$109</definedName>
+    <definedName name="userPlaneDataInterfaceName">Datafill!$B$45</definedName>
+    <definedName name="vSwitchACCESSPortAlias">Datafill!$B$19</definedName>
+    <definedName name="vSwitchACCESSPortName">Datafill!$B$18</definedName>
+    <definedName name="vSwitchDATAPortAlias">Datafill!$B$21</definedName>
+    <definedName name="vSwitchDATAPortName">Datafill!$B$20</definedName>
+    <definedName name="vSwitchMgmtPortAlias">Datafill!$B$15</definedName>
+    <definedName name="vSwitchMgmtPortName">Datafill!$B$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="294">
   <si>
     <t>ASEip</t>
   </si>
@@ -1026,6 +1026,12 @@
   </si>
   <si>
     <t>Other potential DNN's/APN information</t>
+  </si>
+  <si>
+    <t>skipLogin</t>
+  </si>
+  <si>
+    <t>Only for Development or CI/CD environments - Whether to skip interactive login e.g., for when running via pipeline. Always no for typical lab or production setups</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1095,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1208,11 +1214,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1267,6 +1284,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1515,8 +1536,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4718049" y="180975"/>
-          <a:ext cx="16017875" cy="7540625"/>
+          <a:off x="4714874" y="184150"/>
+          <a:ext cx="16017875" cy="7673975"/>
           <a:chOff x="4162425" y="600075"/>
           <a:chExt cx="9744075" cy="4714875"/>
         </a:xfrm>
@@ -1678,6 +1699,7 @@
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
               </a:rPr>
+              <a:pPr algn="ctr"/>
               <a:t>Port2
 IP: 10.214.5.20</a:t>
             </a:fld>
@@ -4619,8 +4641,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FC1B7645-8705-4CBC-9779-7BAA46C774AA}" name="tAutoCfgData" displayName="tAutoCfgData" ref="A1:D112" totalsRowShown="0" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="A1:D112" xr:uid="{FC1B7645-8705-4CBC-9779-7BAA46C774AA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FC1B7645-8705-4CBC-9779-7BAA46C774AA}" name="tAutoCfgData" displayName="tAutoCfgData" ref="A1:D113" totalsRowShown="0" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="A1:D113" xr:uid="{FC1B7645-8705-4CBC-9779-7BAA46C774AA}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{84A6B7EF-69F2-4259-A60E-84BB5D1D43C3}" name="Parameter" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{21F823EC-2D57-410F-9C7B-3D6EC2AA8AE1}" name="Value" dataDxfId="5"/>
@@ -4949,13 +4971,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91708E7-F773-49B2-A66D-1FBD5EC3B43B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5023,316 +5045,316 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>155</v>
+      <c r="A5" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="B5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>173</v>
+        <v>5</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>257</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>174</v>
+        <v>4</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>175</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>260</v>
+        <v>174</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>260</v>
+        <v>174</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>258</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>152</v>
+        <v>267</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>152</v>
+        <v>267</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>176</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>106</v>
+        <v>10</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>264</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>160</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="8">
-        <v>1500</v>
-      </c>
-      <c r="C21" s="2">
-        <v>1500</v>
+        <v>109</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>239</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>270</v>
+        <v>18</v>
+      </c>
+      <c r="B22" s="8">
+        <v>1500</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1500</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>286</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>286</v>
+        <v>63</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>269</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>152</v>
+        <v>68</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>287</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>152</v>
@@ -5341,404 +5363,404 @@
         <v>152</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>271</v>
+        <v>66</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>254</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>178</v>
+        <v>285</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="8">
-        <v>222</v>
-      </c>
-      <c r="C31" s="2">
-        <v>222</v>
+        <v>119</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>240</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>82</v>
+        <v>20</v>
+      </c>
+      <c r="B32" s="8">
+        <v>222</v>
+      </c>
+      <c r="C32" s="2">
+        <v>222</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>195</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="8">
-        <v>333</v>
-      </c>
-      <c r="C37" s="2">
-        <v>333</v>
+        <v>120</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>241</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>82</v>
+        <v>21</v>
+      </c>
+      <c r="B38" s="8">
+        <v>333</v>
+      </c>
+      <c r="C38" s="2">
+        <v>333</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>195</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>180</v>
+        <v>105</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>88</v>
+        <v>17</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>277</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B45" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>182</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>82</v>
@@ -5747,12 +5769,12 @@
         <v>82</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>82</v>
@@ -5761,12 +5783,12 @@
         <v>82</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>82</v>
@@ -5775,12 +5797,12 @@
         <v>82</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>82</v>
@@ -5789,12 +5811,12 @@
         <v>82</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>82</v>
@@ -5803,12 +5825,12 @@
         <v>82</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>82</v>
@@ -5817,12 +5839,12 @@
         <v>82</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>82</v>
@@ -5831,12 +5853,12 @@
         <v>82</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>82</v>
@@ -5845,12 +5867,12 @@
         <v>82</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>82</v>
@@ -5859,26 +5881,26 @@
         <v>82</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="9" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>151</v>
+        <v>82</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>151</v>
+        <v>82</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>151</v>
@@ -5887,12 +5909,12 @@
         <v>151</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>151</v>
@@ -5901,12 +5923,12 @@
         <v>151</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>151</v>
@@ -5915,12 +5937,12 @@
         <v>151</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>151</v>
@@ -5929,12 +5951,12 @@
         <v>151</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>151</v>
@@ -5943,12 +5965,12 @@
         <v>151</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>151</v>
@@ -5957,12 +5979,12 @@
         <v>151</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>151</v>
@@ -5971,12 +5993,12 @@
         <v>151</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>151</v>
@@ -5985,12 +6007,12 @@
         <v>151</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>151</v>
@@ -5999,166 +6021,166 @@
         <v>151</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="9" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="9" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>150</v>
@@ -6167,12 +6189,12 @@
         <v>150</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>150</v>
@@ -6181,12 +6203,12 @@
         <v>150</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>150</v>
@@ -6195,12 +6217,12 @@
         <v>150</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>150</v>
@@ -6209,12 +6231,12 @@
         <v>150</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>150</v>
@@ -6223,12 +6245,12 @@
         <v>150</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>150</v>
@@ -6237,12 +6259,12 @@
         <v>150</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>150</v>
@@ -6251,12 +6273,12 @@
         <v>150</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>150</v>
@@ -6265,12 +6287,12 @@
         <v>150</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>150</v>
@@ -6279,276 +6301,290 @@
         <v>150</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B95" s="8">
-        <v>666</v>
-      </c>
-      <c r="C95" s="2">
-        <v>666</v>
+        <v>51</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B96" s="8">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C96" s="2">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B97" s="8">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C97" s="2">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B98" s="8">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C98" s="2">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B99" s="8">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C99" s="2">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D99" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B100" s="8">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C100" s="2">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B101" s="8">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C101" s="2">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D101" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B102" s="8">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C102" s="2">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D102" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B103" s="8">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C103" s="2">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D103" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B104" s="8">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C104" s="2">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>89</v>
+        <v>31</v>
+      </c>
+      <c r="B105" s="8">
+        <v>675</v>
+      </c>
+      <c r="C105" s="2">
+        <v>675</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D106" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="9" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>162</v>
+        <v>90</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>162</v>
+        <v>90</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>282</v>
+        <v>256</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D108" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="9" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A112" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B111" s="6" t="s">
+      <c r="B112" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="C111" s="7" t="s">
+      <c r="C112" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="D111" s="10" t="s">
+      <c r="D112" s="10" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A112" s="14" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A113" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B112" s="15" t="s">
+      <c r="B113" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="C112" s="16" t="s">
+      <c r="C113" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="D112" s="17" t="s">
+      <c r="D113" s="17" t="s">
         <v>275</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B8:C8">
+  <conditionalFormatting sqref="B9:C9">
     <cfRule type="containsBlanks" dxfId="2" priority="5">
-      <formula>LEN(TRIM(B8))=0</formula>
+      <formula>LEN(TRIM(B9))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28:C29">
+  <conditionalFormatting sqref="B29:C30">
     <cfRule type="containsBlanks" dxfId="1" priority="3">
-      <formula>LEN(TRIM(B28))=0</formula>
+      <formula>LEN(TRIM(B29))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:C44 B105:C112">
+  <conditionalFormatting sqref="B44:C45 B106:C113">
     <cfRule type="containsBlanks" dxfId="0" priority="6">
-      <formula>LEN(TRIM(B43))=0</formula>
+      <formula>LEN(TRIM(B44))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6564,7 +6600,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated parameters file to clarify the usage of 0 for no vlan tagging scenarios
</commit_message>
<xml_diff>
--- a/parameters_file_single_ASE_AP5GC.xlsx
+++ b/parameters_file_single_ASE_AP5GC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/sudeepch_microsoft_com/Documents/Documents/GitHub/ASE_automation_for_AP5GC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{F3EF7CE0-A92A-4BD7-8994-34C8F583455B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83389669-A311-4D6D-A464-79E4E73ED8C8}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{F3EF7CE0-A92A-4BD7-8994-34C8F583455B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E656500D-4EE1-48F9-9CDD-71430475624C}"/>
   <bookViews>
     <workbookView xWindow="37320" yWindow="3045" windowWidth="38640" windowHeight="21120" xr2:uid="{54FBBA50-3CB6-49FD-BB52-63DFE9B337B6}"/>
   </bookViews>
@@ -878,36 +878,6 @@
     <t>Optional VLAN identifier for traffic on the N3 (S1-U) Access network. Leave blank if not in use.</t>
   </si>
   <si>
-    <t>Optional VLAN identifier for traffic on the first N6 (SGi) Data network. Leave blank if not in use.</t>
-  </si>
-  <si>
-    <t>Optional VLAN identifier for traffic on the second N6 (SGi) Data network. Leave blank if not in use.</t>
-  </si>
-  <si>
-    <t>Optional VLAN identifier for traffic on the third N6 (SGi) Data network. Leave blank if not in use.</t>
-  </si>
-  <si>
-    <t>Optional VLAN identifier for traffic on the fourth N6 (SGi) Data network. Leave blank if not in use.</t>
-  </si>
-  <si>
-    <t>Optional VLAN identifier for traffic on the fifth N6 (SGi) Data network. Leave blank if not in use.</t>
-  </si>
-  <si>
-    <t>Optional VLAN identifier for traffic on the sixth N6 (SGi) Data network. Leave blank if not in use.</t>
-  </si>
-  <si>
-    <t>Optional VLAN identifier for traffic on the seventh N6 (SGi) Data network. Leave blank if not in use.</t>
-  </si>
-  <si>
-    <t>Optional VLAN identifier for traffic on the eighth N6 (SGi) Data network. Leave blank if not in use.</t>
-  </si>
-  <si>
-    <t>Optional VLAN identifier for traffic on the ninth N6 (SGi) Data network. Leave blank if not in use.</t>
-  </si>
-  <si>
-    <t>Optional VLAN identifier for traffic on the tenth N6 (SGi) Data network. Leave blank if not in use.</t>
-  </si>
-  <si>
     <t>Mobile Country Code, as defined by ITU. For private testing, 999 is acceptable. Make sure the value selected is approved by your local regulator and compatible with the devices you will be using.</t>
   </si>
   <si>
@@ -1032,6 +1002,36 @@
   </si>
   <si>
     <t>Only for Development or CI/CD environments - Whether to skip interactive login e.g., for when running via pipeline. Always no for typical lab or production setups</t>
+  </si>
+  <si>
+    <t>VLAN identifier for traffic on the first N6 (SGi) Data network. Use value as 0 if you don't plan on implementing vlan tagging on the ASE. Do not leave Blank.</t>
+  </si>
+  <si>
+    <t>Optional VLAN identifier for traffic on the second N6 (SGi) Data network. Use value as 0 if you don't plan on implementing vlan tagging on the ASE. If you do not need this DNN/APN, leave the cell empty.</t>
+  </si>
+  <si>
+    <t>Optional VLAN identifier for traffic on the third N6 (SGi) Data network. Use value as 0 if you don't plan on implementing vlan tagging on the ASE. If you do not need this DNN/APN, leave the cell empty.</t>
+  </si>
+  <si>
+    <t>Optional VLAN identifier for traffic on the fourth N6 (SGi) Data network. Use value as 0 if you don't plan on implementing vlan tagging on the ASE. If you do not need this DNN/APN, leave the cell empty.</t>
+  </si>
+  <si>
+    <t>Optional VLAN identifier for traffic on the fifth N6 (SGi) Data network. Use value as 0 if you don't plan on implementing vlan tagging on the ASE. If you do not need this DNN/APN, leave the cell empty.</t>
+  </si>
+  <si>
+    <t>Optional VLAN identifier for traffic on the sixth N6 (SGi) Data network. Use value as 0 if you don't plan on implementing vlan tagging on the ASE. If you do not need this DNN/APN, leave the cell empty.</t>
+  </si>
+  <si>
+    <t>Optional VLAN identifier for traffic on the seventh N6 (SGi) Data network. Use value as 0 if you don't plan on implementing vlan tagging on the ASE. If you do not need this DNN/APN, leave the cell empty.</t>
+  </si>
+  <si>
+    <t>Optional VLAN identifier for traffic on the eighth N6 (SGi) Data network. Use value as 0 if you don't plan on implementing vlan tagging on the ASE. If you do not need this DNN/APN, leave the cell empty.</t>
+  </si>
+  <si>
+    <t>Optional VLAN identifier for traffic on the ninth N6 (SGi) Data network. Use value as 0 if you don't plan on implementing vlan tagging on the ASE. If you do not need this DNN/APN, leave the cell empty.</t>
+  </si>
+  <si>
+    <t>Optional VLAN identifier for traffic on the tenth N6 (SGi) Data network. Use value as 0 if you don't plan on implementing vlan tagging on the ASE. If you do not need this DNN/APN, leave the cell empty.</t>
   </si>
 </sst>
 </file>
@@ -1536,8 +1536,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4714874" y="184150"/>
-          <a:ext cx="16017875" cy="7673975"/>
+          <a:off x="4718049" y="180975"/>
+          <a:ext cx="16017875" cy="7540625"/>
           <a:chOff x="4162425" y="600075"/>
           <a:chExt cx="9744075" cy="4714875"/>
         </a:xfrm>
@@ -4974,10 +4974,10 @@
   <dimension ref="A1:D113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5021,13 +5021,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -5041,12 +5041,12 @@
         <v>1</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="B5" s="6" t="b">
         <v>0</v>
@@ -5055,7 +5055,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -5111,7 +5111,7 @@
         <v>173</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -5133,13 +5133,13 @@
         <v>62</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -5147,13 +5147,13 @@
         <v>19</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -5167,7 +5167,7 @@
         <v>152</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -5265,7 +5265,7 @@
         <v>165</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -5301,13 +5301,13 @@
         <v>65</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -5315,13 +5315,13 @@
         <v>63</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -5329,13 +5329,13 @@
         <v>67</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -5343,13 +5343,13 @@
         <v>68</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -5363,7 +5363,7 @@
         <v>152</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -5377,7 +5377,7 @@
         <v>152</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -5385,13 +5385,13 @@
         <v>69</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -5399,13 +5399,13 @@
         <v>79</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -5601,7 +5601,7 @@
         <v>88</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -5615,7 +5615,7 @@
         <v>87</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
@@ -6329,7 +6329,7 @@
         <v>666</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>242</v>
+        <v>284</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
@@ -6343,7 +6343,7 @@
         <v>667</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>243</v>
+        <v>285</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
@@ -6357,7 +6357,7 @@
         <v>668</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>244</v>
+        <v>286</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
@@ -6371,7 +6371,7 @@
         <v>669</v>
       </c>
       <c r="D99" s="10" t="s">
-        <v>245</v>
+        <v>287</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
@@ -6385,7 +6385,7 @@
         <v>670</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>246</v>
+        <v>288</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
@@ -6399,7 +6399,7 @@
         <v>671</v>
       </c>
       <c r="D101" s="10" t="s">
-        <v>247</v>
+        <v>289</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
@@ -6413,7 +6413,7 @@
         <v>672</v>
       </c>
       <c r="D102" s="10" t="s">
-        <v>248</v>
+        <v>290</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
@@ -6427,7 +6427,7 @@
         <v>673</v>
       </c>
       <c r="D103" s="10" t="s">
-        <v>249</v>
+        <v>291</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
@@ -6441,7 +6441,7 @@
         <v>674</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>250</v>
+        <v>292</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
@@ -6455,7 +6455,7 @@
         <v>675</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>251</v>
+        <v>293</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
@@ -6469,7 +6469,7 @@
         <v>89</v>
       </c>
       <c r="D106" s="10" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
@@ -6483,7 +6483,7 @@
         <v>90</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
@@ -6497,7 +6497,7 @@
         <v>162</v>
       </c>
       <c r="D108" s="10" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
@@ -6511,7 +6511,7 @@
         <v>163</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
@@ -6525,7 +6525,7 @@
         <v>83</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
@@ -6539,7 +6539,7 @@
         <v>84</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
@@ -6547,13 +6547,13 @@
         <v>72</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="D112" s="10" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
@@ -6561,13 +6561,13 @@
         <v>73</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C113" s="16" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="D113" s="17" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -6742,22 +6742,22 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated parameters file to clarify the usage of 0 for no vlan tagging scenarios for N2 and N3 interfaces
</commit_message>
<xml_diff>
--- a/parameters_file_single_ASE_AP5GC.xlsx
+++ b/parameters_file_single_ASE_AP5GC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/sudeepch_microsoft_com/Documents/Documents/GitHub/ASE_automation_for_AP5GC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{F3EF7CE0-A92A-4BD7-8994-34C8F583455B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E656500D-4EE1-48F9-9CDD-71430475624C}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{F3EF7CE0-A92A-4BD7-8994-34C8F583455B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{160752DB-82F6-4973-9A2A-FAB8875F5291}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="3045" windowWidth="38640" windowHeight="21120" xr2:uid="{54FBBA50-3CB6-49FD-BB52-63DFE9B337B6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{54FBBA50-3CB6-49FD-BB52-63DFE9B337B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Datafill" sheetId="1" r:id="rId1"/>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="293">
   <si>
     <t>ASEip</t>
   </si>
@@ -872,12 +872,6 @@
     <t>Maximum Transmission Unit for the ports of the ASE, in bytes. Values over 1500 are not supported.</t>
   </si>
   <si>
-    <t>Optional VLAN identifier for traffic on the N2 (S1-MME) Access network. Leave blank if not in use.</t>
-  </si>
-  <si>
-    <t>Optional VLAN identifier for traffic on the N3 (S1-U) Access network. Leave blank if not in use.</t>
-  </si>
-  <si>
     <t>Mobile Country Code, as defined by ITU. For private testing, 999 is acceptable. Make sure the value selected is approved by your local regulator and compatible with the devices you will be using.</t>
   </si>
   <si>
@@ -911,9 +905,6 @@
     <t>&lt;cw44ce3FG%gce^3lj5FGD_4&gt;</t>
   </si>
   <si>
-    <t>Enter the ASE password used when connecting to the local setup GUI on ASE</t>
-  </si>
-  <si>
     <t>Name of vswitch to allocate for your DATA port - keep it in the fomat vswitch-Port# format, where # = your DATA port number. Tip: On ASE Pro 2, the Data port is typically 4; on Pro 1, it is "6".</t>
   </si>
   <si>
@@ -1032,6 +1023,12 @@
   </si>
   <si>
     <t>Optional VLAN identifier for traffic on the tenth N6 (SGi) Data network. Use value as 0 if you don't plan on implementing vlan tagging on the ASE. If you do not need this DNN/APN, leave the cell empty.</t>
+  </si>
+  <si>
+    <t>VLAN identifier for traffic on the N3 (S1-U) Access network.  Use value as 0 if you don't plan on implementing vlan tagging on the ASE. Do not leave Blank.</t>
+  </si>
+  <si>
+    <t>Enter the ASE password used when connecting to the local setup GUI on ASE. Don't add any extra characters other than just the full password.</t>
   </si>
 </sst>
 </file>
@@ -1536,8 +1533,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4718049" y="180975"/>
-          <a:ext cx="16017875" cy="7540625"/>
+          <a:off x="4714874" y="184150"/>
+          <a:ext cx="16017875" cy="7673975"/>
           <a:chOff x="4162425" y="600075"/>
           <a:chExt cx="9744075" cy="4714875"/>
         </a:xfrm>
@@ -4974,10 +4971,10 @@
   <dimension ref="A1:D113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D43" sqref="D43"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5021,13 +5018,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>253</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -5041,12 +5038,12 @@
         <v>1</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B5" s="6" t="b">
         <v>0</v>
@@ -5055,7 +5052,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -5111,7 +5108,7 @@
         <v>173</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -5133,13 +5130,13 @@
         <v>62</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -5147,13 +5144,13 @@
         <v>19</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -5167,7 +5164,7 @@
         <v>152</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -5265,7 +5262,7 @@
         <v>165</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -5301,13 +5298,13 @@
         <v>65</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -5315,13 +5312,13 @@
         <v>63</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -5329,13 +5326,13 @@
         <v>67</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -5343,13 +5340,13 @@
         <v>68</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -5363,7 +5360,7 @@
         <v>152</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -5377,7 +5374,7 @@
         <v>152</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -5385,13 +5382,13 @@
         <v>69</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -5399,13 +5396,13 @@
         <v>79</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -5433,7 +5430,7 @@
         <v>222</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>240</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -5517,7 +5514,7 @@
         <v>333</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>241</v>
+        <v>291</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -5601,7 +5598,7 @@
         <v>88</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -5615,7 +5612,7 @@
         <v>87</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
@@ -6329,7 +6326,7 @@
         <v>666</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
@@ -6343,7 +6340,7 @@
         <v>667</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
@@ -6357,7 +6354,7 @@
         <v>668</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
@@ -6371,7 +6368,7 @@
         <v>669</v>
       </c>
       <c r="D99" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
@@ -6385,7 +6382,7 @@
         <v>670</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
@@ -6399,7 +6396,7 @@
         <v>671</v>
       </c>
       <c r="D101" s="10" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
@@ -6413,7 +6410,7 @@
         <v>672</v>
       </c>
       <c r="D102" s="10" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
@@ -6427,7 +6424,7 @@
         <v>673</v>
       </c>
       <c r="D103" s="10" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
@@ -6441,7 +6438,7 @@
         <v>674</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
@@ -6455,7 +6452,7 @@
         <v>675</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
@@ -6469,7 +6466,7 @@
         <v>89</v>
       </c>
       <c r="D106" s="10" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
@@ -6483,7 +6480,7 @@
         <v>90</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
@@ -6497,7 +6494,7 @@
         <v>162</v>
       </c>
       <c r="D108" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
@@ -6511,7 +6508,7 @@
         <v>163</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
@@ -6525,7 +6522,7 @@
         <v>83</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
@@ -6539,7 +6536,7 @@
         <v>84</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
@@ -6547,13 +6544,13 @@
         <v>72</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D112" s="10" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
@@ -6561,13 +6558,13 @@
         <v>73</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C113" s="16" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D113" s="17" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -6742,22 +6739,22 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
minor interface name typo correction in comments section of parameters file
</commit_message>
<xml_diff>
--- a/parameters_file_single_ASE_AP5GC.xlsx
+++ b/parameters_file_single_ASE_AP5GC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/sudeepch_microsoft_com/Documents/Documents/GitHub/ASE_automation_for_AP5GC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{F3EF7CE0-A92A-4BD7-8994-34C8F583455B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{160752DB-82F6-4973-9A2A-FAB8875F5291}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{F3EF7CE0-A92A-4BD7-8994-34C8F583455B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC40C48C-42D4-4D34-99DC-82EEC39FA03C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{54FBBA50-3CB6-49FD-BB52-63DFE9B337B6}"/>
   </bookViews>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="294">
   <si>
     <t>ASEip</t>
   </si>
@@ -1029,6 +1029,9 @@
   </si>
   <si>
     <t>Enter the ASE password used when connecting to the local setup GUI on ASE. Don't add any extra characters other than just the full password.</t>
+  </si>
+  <si>
+    <t>VLAN identifier for traffic on the N2 (S1-MME) Access network.  Use value as 0 if you don't plan on implementing vlan tagging on the ASE. Do not leave Blank.</t>
   </si>
 </sst>
 </file>
@@ -4971,10 +4974,10 @@
   <dimension ref="A1:D113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D72" sqref="D72"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5430,7 +5433,7 @@
         <v>222</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>